<commit_message>
Ajout des librairies apres les avoir combiné
</commit_message>
<xml_diff>
--- a/Index Produits/INDEX_EQUIPE_ILYES_CAMILLE.xlsx
+++ b/Index Produits/INDEX_EQUIPE_ILYES_CAMILLE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Projet de fin de DEC\SecurityDoor\Index Produits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projet\SecurityDoor\Index Produits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8899210-7C81-406E-817E-6313DAF752D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D3C072-EA5D-4FF3-ADA1-62081261BC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LISTE" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="425">
   <si>
     <t>Catégorie</t>
   </si>
@@ -1261,13 +1261,64 @@
   </si>
   <si>
     <t>CAP CER 22nF 15V 10% 0603, X7R</t>
+  </si>
+  <si>
+    <t>E00077</t>
+  </si>
+  <si>
+    <t>Diodes TVS</t>
+  </si>
+  <si>
+    <t>CPDQ5V0-HF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diode TVS </t>
+  </si>
+  <si>
+    <t>Comchip</t>
+  </si>
+  <si>
+    <t>E00081</t>
+  </si>
+  <si>
+    <t>0ZCJ0100FF2E</t>
+  </si>
+  <si>
+    <t>Polyswitch</t>
+  </si>
+  <si>
+    <t>Bel Fuse Inc</t>
+  </si>
+  <si>
+    <t>E00082</t>
+  </si>
+  <si>
+    <t>SSM3J130TU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transistor </t>
+  </si>
+  <si>
+    <t>Mosfet P 20V 4.4A</t>
+  </si>
+  <si>
+    <t>Toshiba</t>
+  </si>
+  <si>
+    <t>E00083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bipolaire NPN </t>
+  </si>
+  <si>
+    <t>MMBT2222ATT1G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1295,6 +1346,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1390,7 +1447,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1478,12 +1535,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2220,8 +2287,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E488228-7BB2-48E8-8D64-0FE9665C033D}" name="Tableau13" displayName="Tableau13" ref="A5:M86" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A5:M86" xr:uid="{58943F4C-4DE4-4629-A635-9F2408F28BF2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E488228-7BB2-48E8-8D64-0FE9665C033D}" name="Tableau13" displayName="Tableau13" ref="A5:M90" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A5:M90" xr:uid="{58943F4C-4DE4-4629-A635-9F2408F28BF2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:M86">
     <sortCondition ref="A10:A86"/>
   </sortState>
@@ -2567,28 +2634,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="D80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="33.85546875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="9.59765625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.3984375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.3984375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="38.1328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.59765625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.73046875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="22.1328125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="25.1328125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="33.86328125" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.3984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -2607,7 +2674,7 @@
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2618,7 +2685,7 @@
       <c r="D2" s="11"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -2635,10 +2702,10 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="8"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
         <v>50</v>
       </c>
@@ -2679,7 +2746,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
         <v>62</v>
       </c>
@@ -2714,7 +2781,7 @@
       </c>
       <c r="M6" s="21"/>
     </row>
-    <row r="7" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>74</v>
       </c>
@@ -2749,7 +2816,7 @@
       </c>
       <c r="M7" s="21"/>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>75</v>
       </c>
@@ -2786,7 +2853,7 @@
       </c>
       <c r="M8" s="21"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>76</v>
       </c>
@@ -2821,7 +2888,7 @@
       </c>
       <c r="M9" s="21"/>
     </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="16" t="s">
         <v>77</v>
       </c>
@@ -2856,7 +2923,7 @@
       </c>
       <c r="M10" s="21"/>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
         <v>78</v>
       </c>
@@ -2891,7 +2958,7 @@
       </c>
       <c r="M11" s="21"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
         <v>79</v>
       </c>
@@ -2928,7 +2995,7 @@
       </c>
       <c r="M12" s="21"/>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="16" t="s">
         <v>80</v>
       </c>
@@ -2965,7 +3032,7 @@
       </c>
       <c r="M13" s="21"/>
     </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="16" t="s">
         <v>81</v>
       </c>
@@ -3002,7 +3069,7 @@
       </c>
       <c r="M14" s="21"/>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="30" t="s">
         <v>82</v>
       </c>
@@ -3039,7 +3106,7 @@
       </c>
       <c r="M15" s="21"/>
     </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
         <v>83</v>
       </c>
@@ -3076,7 +3143,7 @@
       </c>
       <c r="M16" s="21"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="16" t="s">
         <v>84</v>
       </c>
@@ -3113,7 +3180,7 @@
       </c>
       <c r="M17" s="21"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="16" t="s">
         <v>85</v>
       </c>
@@ -3150,7 +3217,7 @@
       </c>
       <c r="M18" s="21"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
         <v>86</v>
       </c>
@@ -3185,7 +3252,7 @@
       </c>
       <c r="M19" s="21"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="16" t="s">
         <v>87</v>
       </c>
@@ -3222,7 +3289,7 @@
       </c>
       <c r="M20" s="21"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="16" t="s">
         <v>88</v>
       </c>
@@ -3259,7 +3326,7 @@
       </c>
       <c r="M21" s="21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>89</v>
       </c>
@@ -3296,7 +3363,7 @@
       </c>
       <c r="M22" s="21"/>
     </row>
-    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" s="16" t="s">
         <v>90</v>
       </c>
@@ -3333,7 +3400,7 @@
       </c>
       <c r="M23" s="21"/>
     </row>
-    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="16" t="s">
         <v>91</v>
       </c>
@@ -3368,7 +3435,7 @@
       </c>
       <c r="M24" s="21"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="16" t="s">
         <v>92</v>
       </c>
@@ -3405,7 +3472,7 @@
       </c>
       <c r="M25" s="21"/>
     </row>
-    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>140</v>
       </c>
@@ -3444,7 +3511,7 @@
       </c>
       <c r="M26" s="21"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="16" t="s">
         <v>141</v>
       </c>
@@ -3481,7 +3548,7 @@
       </c>
       <c r="M27" s="21"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
         <v>93</v>
       </c>
@@ -3518,7 +3585,7 @@
       </c>
       <c r="M28" s="21"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="16" t="s">
         <v>94</v>
       </c>
@@ -3555,7 +3622,7 @@
       </c>
       <c r="M29" s="21"/>
     </row>
-    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30" s="16" t="s">
         <v>95</v>
       </c>
@@ -3592,7 +3659,7 @@
       </c>
       <c r="M30" s="21"/>
     </row>
-    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="16" t="s">
         <v>96</v>
       </c>
@@ -3629,7 +3696,7 @@
       </c>
       <c r="M31" s="21"/>
     </row>
-    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="16" t="s">
         <v>97</v>
       </c>
@@ -3666,7 +3733,7 @@
       </c>
       <c r="M32" s="21"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="16" t="s">
         <v>98</v>
       </c>
@@ -3703,7 +3770,7 @@
       </c>
       <c r="M33" s="21"/>
     </row>
-    <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="13" t="s">
         <v>67</v>
       </c>
@@ -3740,7 +3807,7 @@
       </c>
       <c r="M34" s="21"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="16" t="s">
         <v>99</v>
       </c>
@@ -3775,7 +3842,7 @@
       </c>
       <c r="M35" s="21"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="16" t="s">
         <v>100</v>
       </c>
@@ -3810,7 +3877,7 @@
       </c>
       <c r="M36" s="21"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="16" t="s">
         <v>101</v>
       </c>
@@ -3845,7 +3912,7 @@
       </c>
       <c r="M37" s="21"/>
     </row>
-    <row r="38" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A38" s="16" t="s">
         <v>102</v>
       </c>
@@ -3880,7 +3947,7 @@
       </c>
       <c r="M38" s="21"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" s="16" t="s">
         <v>103</v>
       </c>
@@ -3915,7 +3982,7 @@
       </c>
       <c r="M39" s="21"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" s="16" t="s">
         <v>104</v>
       </c>
@@ -3948,7 +4015,7 @@
       </c>
       <c r="M40" s="21"/>
     </row>
-    <row r="41" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A41" s="16" t="s">
         <v>105</v>
       </c>
@@ -3983,7 +4050,7 @@
       </c>
       <c r="M41" s="21"/>
     </row>
-    <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A42" s="16" t="s">
         <v>106</v>
       </c>
@@ -4018,7 +4085,7 @@
       </c>
       <c r="M42" s="21"/>
     </row>
-    <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" s="16" t="s">
         <v>107</v>
       </c>
@@ -4053,7 +4120,7 @@
       </c>
       <c r="M43" s="21"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44" s="16" t="s">
         <v>108</v>
       </c>
@@ -4090,7 +4157,7 @@
       </c>
       <c r="M44" s="21"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A45" s="16" t="s">
         <v>109</v>
       </c>
@@ -4127,7 +4194,7 @@
       </c>
       <c r="M45" s="21"/>
     </row>
-    <row r="46" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A46" s="16" t="s">
         <v>110</v>
       </c>
@@ -4162,7 +4229,7 @@
       </c>
       <c r="M46" s="21"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A47" s="16" t="s">
         <v>111</v>
       </c>
@@ -4199,7 +4266,7 @@
       </c>
       <c r="M47" s="21"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A48" s="16" t="s">
         <v>112</v>
       </c>
@@ -4236,7 +4303,7 @@
       </c>
       <c r="M48" s="21"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A49" s="16" t="s">
         <v>113</v>
       </c>
@@ -4271,7 +4338,7 @@
       </c>
       <c r="M49" s="21"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A50" s="16" t="s">
         <v>114</v>
       </c>
@@ -4306,7 +4373,7 @@
       </c>
       <c r="M50" s="21"/>
     </row>
-    <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A51" s="16" t="s">
         <v>115</v>
       </c>
@@ -4343,7 +4410,7 @@
       </c>
       <c r="M51" s="21"/>
     </row>
-    <row r="52" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A52" s="16" t="s">
         <v>116</v>
       </c>
@@ -4376,7 +4443,7 @@
       </c>
       <c r="M52" s="21"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A53" s="16" t="s">
         <v>117</v>
       </c>
@@ -4411,7 +4478,7 @@
       </c>
       <c r="M53" s="21"/>
     </row>
-    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A54" s="16" t="s">
         <v>118</v>
       </c>
@@ -4448,7 +4515,7 @@
       </c>
       <c r="M54" s="21"/>
     </row>
-    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A55" s="16" t="s">
         <v>119</v>
       </c>
@@ -4485,7 +4552,7 @@
       </c>
       <c r="M55" s="21"/>
     </row>
-    <row r="56" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A56" s="16" t="s">
         <v>120</v>
       </c>
@@ -4522,7 +4589,7 @@
       </c>
       <c r="M56" s="21"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A57" s="16" t="s">
         <v>73</v>
       </c>
@@ -4557,7 +4624,7 @@
       </c>
       <c r="M57" s="21"/>
     </row>
-    <row r="58" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A58" s="16" t="s">
         <v>121</v>
       </c>
@@ -4594,7 +4661,7 @@
       </c>
       <c r="M58" s="21"/>
     </row>
-    <row r="59" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A59" s="16" t="s">
         <v>122</v>
       </c>
@@ -4631,7 +4698,7 @@
       </c>
       <c r="M59" s="21"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A60" s="16" t="s">
         <v>123</v>
       </c>
@@ -4668,7 +4735,7 @@
       </c>
       <c r="M60" s="21"/>
     </row>
-    <row r="61" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A61" s="16" t="s">
         <v>124</v>
       </c>
@@ -4705,7 +4772,7 @@
       </c>
       <c r="M61" s="21"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A62" s="16" t="s">
         <v>125</v>
       </c>
@@ -4742,7 +4809,7 @@
       </c>
       <c r="M62" s="21"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A63" s="16" t="s">
         <v>126</v>
       </c>
@@ -4779,7 +4846,7 @@
       </c>
       <c r="M63" s="21"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A64" s="13" t="s">
         <v>127</v>
       </c>
@@ -4816,7 +4883,7 @@
       </c>
       <c r="M64" s="21"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A65" s="16" t="s">
         <v>128</v>
       </c>
@@ -4853,7 +4920,7 @@
       </c>
       <c r="M65" s="21"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A66" s="16" t="s">
         <v>129</v>
       </c>
@@ -4890,7 +4957,7 @@
       </c>
       <c r="M66" s="21"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A67" s="16" t="s">
         <v>130</v>
       </c>
@@ -4927,7 +4994,7 @@
       </c>
       <c r="M67" s="21"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A68" s="16" t="s">
         <v>131</v>
       </c>
@@ -4964,7 +5031,7 @@
       </c>
       <c r="M68" s="21"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A69" s="13" t="s">
         <v>132</v>
       </c>
@@ -4999,7 +5066,7 @@
       </c>
       <c r="M69" s="21"/>
     </row>
-    <row r="70" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A70" s="16" t="s">
         <v>133</v>
       </c>
@@ -5032,7 +5099,7 @@
       </c>
       <c r="M70" s="21"/>
     </row>
-    <row r="71" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="16" t="s">
         <v>134</v>
       </c>
@@ -5069,7 +5136,7 @@
       </c>
       <c r="M71" s="21"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A72" s="16" t="s">
         <v>135</v>
       </c>
@@ -5106,7 +5173,7 @@
       </c>
       <c r="M72" s="21"/>
     </row>
-    <row r="73" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A73" s="16" t="s">
         <v>136</v>
       </c>
@@ -5143,7 +5210,7 @@
       </c>
       <c r="M73" s="21"/>
     </row>
-    <row r="74" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A74" s="16" t="s">
         <v>137</v>
       </c>
@@ -5180,7 +5247,7 @@
       </c>
       <c r="M74" s="21"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A75" s="16" t="s">
         <v>138</v>
       </c>
@@ -5217,7 +5284,7 @@
       </c>
       <c r="M75" s="21"/>
     </row>
-    <row r="76" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A76" s="16" t="s">
         <v>139</v>
       </c>
@@ -5252,7 +5319,7 @@
       </c>
       <c r="M76" s="21"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A77" s="13" t="s">
         <v>142</v>
       </c>
@@ -5291,7 +5358,7 @@
       </c>
       <c r="M77" s="21"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A78" s="13" t="s">
         <v>143</v>
       </c>
@@ -5330,7 +5397,7 @@
       </c>
       <c r="M78" s="21"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A79" s="13" t="s">
         <v>144</v>
       </c>
@@ -5363,7 +5430,7 @@
       </c>
       <c r="M79" s="21"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A80" s="13" t="s">
         <v>145</v>
       </c>
@@ -5398,7 +5465,7 @@
       </c>
       <c r="M80" s="21"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A81" s="13" t="s">
         <v>146</v>
       </c>
@@ -5414,7 +5481,7 @@
       <c r="E81" s="17" t="s">
         <v>406</v>
       </c>
-      <c r="F81" s="32"/>
+      <c r="F81" s="6"/>
       <c r="G81" s="15" t="s">
         <v>146</v>
       </c>
@@ -5433,7 +5500,7 @@
       </c>
       <c r="M81" s="21"/>
     </row>
-    <row r="82" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A82" s="13" t="s">
         <v>147</v>
       </c>
@@ -5470,7 +5537,7 @@
       </c>
       <c r="M82" s="21"/>
     </row>
-    <row r="83" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A83" s="13" t="s">
         <v>148</v>
       </c>
@@ -5505,7 +5572,7 @@
       </c>
       <c r="M83" s="21"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A84" s="13" t="s">
         <v>149</v>
       </c>
@@ -5538,7 +5605,7 @@
       </c>
       <c r="M84" s="21"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A85" s="28" t="s">
         <v>400</v>
       </c>
@@ -5567,7 +5634,7 @@
       <c r="L85" s="24"/>
       <c r="M85" s="23"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A86" s="28" t="s">
         <v>399</v>
       </c>
@@ -5597,13 +5664,141 @@
       <c r="L86" s="24"/>
       <c r="M86" s="23"/>
     </row>
-    <row r="99" spans="1:13" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="1:13" ht="20.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A87" s="32" t="s">
+        <v>408</v>
+      </c>
+      <c r="B87" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" s="24" t="s">
+        <v>409</v>
+      </c>
+      <c r="D87" s="34" t="s">
+        <v>410</v>
+      </c>
+      <c r="E87" s="33" t="s">
+        <v>411</v>
+      </c>
+      <c r="F87" s="33" t="s">
+        <v>412</v>
+      </c>
+      <c r="G87" s="25" t="s">
+        <v>408</v>
+      </c>
+      <c r="H87" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I87" s="25"/>
+      <c r="J87" s="25"/>
+      <c r="K87" s="33"/>
+      <c r="L87" s="24"/>
+      <c r="M87" s="23"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A88" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="B88" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="D88" s="34" t="s">
+        <v>414</v>
+      </c>
+      <c r="E88" s="33" t="s">
+        <v>415</v>
+      </c>
+      <c r="F88" s="33" t="s">
+        <v>416</v>
+      </c>
+      <c r="G88" s="35" t="s">
+        <v>413</v>
+      </c>
+      <c r="H88" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I88" s="25"/>
+      <c r="J88" s="25"/>
+      <c r="K88" s="33"/>
+      <c r="L88" s="34" t="s">
+        <v>414</v>
+      </c>
+      <c r="M88" s="23"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A89" s="32" t="s">
+        <v>417</v>
+      </c>
+      <c r="B89" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="24" t="s">
+        <v>419</v>
+      </c>
+      <c r="D89" s="36" t="s">
+        <v>418</v>
+      </c>
+      <c r="E89" s="33" t="s">
+        <v>420</v>
+      </c>
+      <c r="F89" s="33" t="s">
+        <v>421</v>
+      </c>
+      <c r="G89" s="35" t="s">
+        <v>417</v>
+      </c>
+      <c r="H89" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I89" s="25"/>
+      <c r="J89" s="25"/>
+      <c r="K89" s="33"/>
+      <c r="L89" s="36" t="s">
+        <v>418</v>
+      </c>
+      <c r="M89" s="23"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A90" s="32" t="s">
+        <v>422</v>
+      </c>
+      <c r="B90" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="24" t="s">
+        <v>419</v>
+      </c>
+      <c r="D90" s="34" t="s">
+        <v>424</v>
+      </c>
+      <c r="E90" s="33" t="s">
+        <v>423</v>
+      </c>
+      <c r="F90" s="33"/>
+      <c r="G90" s="35" t="s">
+        <v>422</v>
+      </c>
+      <c r="H90" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I90" s="25"/>
+      <c r="J90" s="25"/>
+      <c r="K90" s="33"/>
+      <c r="L90" s="24" t="s">
+        <v>424</v>
+      </c>
+      <c r="M90" s="23"/>
+    </row>
+    <row r="99" spans="1:13" ht="54.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="100" spans="1:13" ht="20.45" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="101" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="102" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="103" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="104" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="107" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="2"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -5618,8 +5813,8 @@
       <c r="L107" s="3"/>
       <c r="M107" s="3"/>
     </row>
-    <row r="108" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="109" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="2"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -5634,8 +5829,8 @@
       <c r="L109" s="3"/>
       <c r="M109" s="3"/>
     </row>
-    <row r="110" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="111" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="2"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -5650,7 +5845,7 @@
       <c r="L111" s="3"/>
       <c r="M111" s="3"/>
     </row>
-    <row r="113" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="2"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -5665,7 +5860,7 @@
       <c r="L113" s="3"/>
       <c r="M113" s="3"/>
     </row>
-    <row r="115" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115" s="2"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -5680,8 +5875,8 @@
       <c r="L115" s="3"/>
       <c r="M115" s="3"/>
     </row>
-    <row r="116" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="117" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A117" s="2"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -5696,12 +5891,12 @@
       <c r="L117" s="3"/>
       <c r="M117" s="3"/>
     </row>
-    <row r="118" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="130" ht="12.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="131" ht="12.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="132" ht="12.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="133" ht="12.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="134" ht="14.1" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -5786,11 +5981,12 @@
     <hyperlink ref="G82" r:id="rId79" xr:uid="{02A4A74A-7559-4FE0-B02B-DAE20A0CEEA4}"/>
     <hyperlink ref="G83" r:id="rId80" xr:uid="{5C207BBA-BB55-4CA1-A138-D0BC7ED18D62}"/>
     <hyperlink ref="G84" r:id="rId81" xr:uid="{551B6000-23BB-462B-9430-7BF1BF6FD608}"/>
+    <hyperlink ref="G87" r:id="rId82" xr:uid="{C38B4FA5-EC5E-4508-A2ED-EB99F2774757}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId82"/>
+  <pageSetup orientation="portrait" r:id="rId83"/>
   <tableParts count="1">
-    <tablePart r:id="rId83"/>
+    <tablePart r:id="rId84"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5803,14 +5999,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.265625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -5822,7 +6018,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5833,7 +6029,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -5844,7 +6040,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -5855,7 +6051,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -5866,7 +6062,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -5877,7 +6073,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -5888,7 +6084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -5899,7 +6095,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -5910,7 +6106,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -5921,7 +6117,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -5932,82 +6128,82 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -6026,12 +6222,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>

<commit_message>
Commit juste pour etre capable de merge AVEC LE MAIN
</commit_message>
<xml_diff>
--- a/Index Produits/INDEX_EQUIPE_ILYES_CAMILLE.xlsx
+++ b/Index Produits/INDEX_EQUIPE_ILYES_CAMILLE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Projet de fin de DEC\SecurityDoor\Index Produits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projet\SecurityDoor\Index Produits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8899210-7C81-406E-817E-6313DAF752D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6394CBA-AF55-44E5-BD49-659322738331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LISTE" sheetId="1" r:id="rId1"/>
@@ -1390,7 +1390,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1478,10 +1478,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2567,28 +2564,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F89" sqref="F88:F89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="33.85546875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="9.59765625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.3984375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.3984375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="38.1328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.59765625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.73046875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="22.1328125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="25.1328125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="33.86328125" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.3984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -2607,7 +2604,7 @@
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2618,7 +2615,7 @@
       <c r="D2" s="11"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -2635,10 +2632,10 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="8"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
         <v>50</v>
       </c>
@@ -2679,7 +2676,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
         <v>62</v>
       </c>
@@ -2714,7 +2711,7 @@
       </c>
       <c r="M6" s="21"/>
     </row>
-    <row r="7" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>74</v>
       </c>
@@ -2749,7 +2746,7 @@
       </c>
       <c r="M7" s="21"/>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>75</v>
       </c>
@@ -2786,7 +2783,7 @@
       </c>
       <c r="M8" s="21"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>76</v>
       </c>
@@ -2821,7 +2818,7 @@
       </c>
       <c r="M9" s="21"/>
     </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="16" t="s">
         <v>77</v>
       </c>
@@ -2856,7 +2853,7 @@
       </c>
       <c r="M10" s="21"/>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
         <v>78</v>
       </c>
@@ -2891,7 +2888,7 @@
       </c>
       <c r="M11" s="21"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
         <v>79</v>
       </c>
@@ -2928,7 +2925,7 @@
       </c>
       <c r="M12" s="21"/>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="16" t="s">
         <v>80</v>
       </c>
@@ -2965,7 +2962,7 @@
       </c>
       <c r="M13" s="21"/>
     </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="16" t="s">
         <v>81</v>
       </c>
@@ -3002,7 +2999,7 @@
       </c>
       <c r="M14" s="21"/>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="30" t="s">
         <v>82</v>
       </c>
@@ -3039,7 +3036,7 @@
       </c>
       <c r="M15" s="21"/>
     </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
         <v>83</v>
       </c>
@@ -3076,7 +3073,7 @@
       </c>
       <c r="M16" s="21"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="16" t="s">
         <v>84</v>
       </c>
@@ -3113,7 +3110,7 @@
       </c>
       <c r="M17" s="21"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="16" t="s">
         <v>85</v>
       </c>
@@ -3150,7 +3147,7 @@
       </c>
       <c r="M18" s="21"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
         <v>86</v>
       </c>
@@ -3185,7 +3182,7 @@
       </c>
       <c r="M19" s="21"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="16" t="s">
         <v>87</v>
       </c>
@@ -3222,7 +3219,7 @@
       </c>
       <c r="M20" s="21"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="16" t="s">
         <v>88</v>
       </c>
@@ -3259,7 +3256,7 @@
       </c>
       <c r="M21" s="21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>89</v>
       </c>
@@ -3296,7 +3293,7 @@
       </c>
       <c r="M22" s="21"/>
     </row>
-    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" s="16" t="s">
         <v>90</v>
       </c>
@@ -3333,7 +3330,7 @@
       </c>
       <c r="M23" s="21"/>
     </row>
-    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="16" t="s">
         <v>91</v>
       </c>
@@ -3368,7 +3365,7 @@
       </c>
       <c r="M24" s="21"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="16" t="s">
         <v>92</v>
       </c>
@@ -3405,7 +3402,7 @@
       </c>
       <c r="M25" s="21"/>
     </row>
-    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>140</v>
       </c>
@@ -3444,7 +3441,7 @@
       </c>
       <c r="M26" s="21"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="16" t="s">
         <v>141</v>
       </c>
@@ -3481,7 +3478,7 @@
       </c>
       <c r="M27" s="21"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
         <v>93</v>
       </c>
@@ -3518,7 +3515,7 @@
       </c>
       <c r="M28" s="21"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="16" t="s">
         <v>94</v>
       </c>
@@ -3555,7 +3552,7 @@
       </c>
       <c r="M29" s="21"/>
     </row>
-    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30" s="16" t="s">
         <v>95</v>
       </c>
@@ -3592,7 +3589,7 @@
       </c>
       <c r="M30" s="21"/>
     </row>
-    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="16" t="s">
         <v>96</v>
       </c>
@@ -3629,7 +3626,7 @@
       </c>
       <c r="M31" s="21"/>
     </row>
-    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="16" t="s">
         <v>97</v>
       </c>
@@ -3666,7 +3663,7 @@
       </c>
       <c r="M32" s="21"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="16" t="s">
         <v>98</v>
       </c>
@@ -3703,7 +3700,7 @@
       </c>
       <c r="M33" s="21"/>
     </row>
-    <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="13" t="s">
         <v>67</v>
       </c>
@@ -3740,7 +3737,7 @@
       </c>
       <c r="M34" s="21"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="16" t="s">
         <v>99</v>
       </c>
@@ -3775,7 +3772,7 @@
       </c>
       <c r="M35" s="21"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="16" t="s">
         <v>100</v>
       </c>
@@ -3810,7 +3807,7 @@
       </c>
       <c r="M36" s="21"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="16" t="s">
         <v>101</v>
       </c>
@@ -3845,7 +3842,7 @@
       </c>
       <c r="M37" s="21"/>
     </row>
-    <row r="38" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A38" s="16" t="s">
         <v>102</v>
       </c>
@@ -3880,7 +3877,7 @@
       </c>
       <c r="M38" s="21"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" s="16" t="s">
         <v>103</v>
       </c>
@@ -3915,7 +3912,7 @@
       </c>
       <c r="M39" s="21"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" s="16" t="s">
         <v>104</v>
       </c>
@@ -3948,7 +3945,7 @@
       </c>
       <c r="M40" s="21"/>
     </row>
-    <row r="41" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A41" s="16" t="s">
         <v>105</v>
       </c>
@@ -3983,7 +3980,7 @@
       </c>
       <c r="M41" s="21"/>
     </row>
-    <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A42" s="16" t="s">
         <v>106</v>
       </c>
@@ -4018,7 +4015,7 @@
       </c>
       <c r="M42" s="21"/>
     </row>
-    <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" s="16" t="s">
         <v>107</v>
       </c>
@@ -4053,7 +4050,7 @@
       </c>
       <c r="M43" s="21"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44" s="16" t="s">
         <v>108</v>
       </c>
@@ -4090,7 +4087,7 @@
       </c>
       <c r="M44" s="21"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A45" s="16" t="s">
         <v>109</v>
       </c>
@@ -4127,7 +4124,7 @@
       </c>
       <c r="M45" s="21"/>
     </row>
-    <row r="46" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A46" s="16" t="s">
         <v>110</v>
       </c>
@@ -4162,7 +4159,7 @@
       </c>
       <c r="M46" s="21"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A47" s="16" t="s">
         <v>111</v>
       </c>
@@ -4199,7 +4196,7 @@
       </c>
       <c r="M47" s="21"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A48" s="16" t="s">
         <v>112</v>
       </c>
@@ -4236,7 +4233,7 @@
       </c>
       <c r="M48" s="21"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A49" s="16" t="s">
         <v>113</v>
       </c>
@@ -4271,7 +4268,7 @@
       </c>
       <c r="M49" s="21"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A50" s="16" t="s">
         <v>114</v>
       </c>
@@ -4306,7 +4303,7 @@
       </c>
       <c r="M50" s="21"/>
     </row>
-    <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A51" s="16" t="s">
         <v>115</v>
       </c>
@@ -4343,7 +4340,7 @@
       </c>
       <c r="M51" s="21"/>
     </row>
-    <row r="52" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A52" s="16" t="s">
         <v>116</v>
       </c>
@@ -4376,7 +4373,7 @@
       </c>
       <c r="M52" s="21"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A53" s="16" t="s">
         <v>117</v>
       </c>
@@ -4411,7 +4408,7 @@
       </c>
       <c r="M53" s="21"/>
     </row>
-    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A54" s="16" t="s">
         <v>118</v>
       </c>
@@ -4448,7 +4445,7 @@
       </c>
       <c r="M54" s="21"/>
     </row>
-    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A55" s="16" t="s">
         <v>119</v>
       </c>
@@ -4485,7 +4482,7 @@
       </c>
       <c r="M55" s="21"/>
     </row>
-    <row r="56" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A56" s="16" t="s">
         <v>120</v>
       </c>
@@ -4522,7 +4519,7 @@
       </c>
       <c r="M56" s="21"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A57" s="16" t="s">
         <v>73</v>
       </c>
@@ -4557,7 +4554,7 @@
       </c>
       <c r="M57" s="21"/>
     </row>
-    <row r="58" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A58" s="16" t="s">
         <v>121</v>
       </c>
@@ -4594,7 +4591,7 @@
       </c>
       <c r="M58" s="21"/>
     </row>
-    <row r="59" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A59" s="16" t="s">
         <v>122</v>
       </c>
@@ -4631,7 +4628,7 @@
       </c>
       <c r="M59" s="21"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A60" s="16" t="s">
         <v>123</v>
       </c>
@@ -4668,7 +4665,7 @@
       </c>
       <c r="M60" s="21"/>
     </row>
-    <row r="61" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A61" s="16" t="s">
         <v>124</v>
       </c>
@@ -4705,7 +4702,7 @@
       </c>
       <c r="M61" s="21"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A62" s="16" t="s">
         <v>125</v>
       </c>
@@ -4742,7 +4739,7 @@
       </c>
       <c r="M62" s="21"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A63" s="16" t="s">
         <v>126</v>
       </c>
@@ -4779,7 +4776,7 @@
       </c>
       <c r="M63" s="21"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A64" s="13" t="s">
         <v>127</v>
       </c>
@@ -4816,7 +4813,7 @@
       </c>
       <c r="M64" s="21"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A65" s="16" t="s">
         <v>128</v>
       </c>
@@ -4853,7 +4850,7 @@
       </c>
       <c r="M65" s="21"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A66" s="16" t="s">
         <v>129</v>
       </c>
@@ -4890,7 +4887,7 @@
       </c>
       <c r="M66" s="21"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A67" s="16" t="s">
         <v>130</v>
       </c>
@@ -4927,7 +4924,7 @@
       </c>
       <c r="M67" s="21"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A68" s="16" t="s">
         <v>131</v>
       </c>
@@ -4964,7 +4961,7 @@
       </c>
       <c r="M68" s="21"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A69" s="13" t="s">
         <v>132</v>
       </c>
@@ -4999,7 +4996,7 @@
       </c>
       <c r="M69" s="21"/>
     </row>
-    <row r="70" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A70" s="16" t="s">
         <v>133</v>
       </c>
@@ -5032,7 +5029,7 @@
       </c>
       <c r="M70" s="21"/>
     </row>
-    <row r="71" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="16" t="s">
         <v>134</v>
       </c>
@@ -5069,7 +5066,7 @@
       </c>
       <c r="M71" s="21"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A72" s="16" t="s">
         <v>135</v>
       </c>
@@ -5106,7 +5103,7 @@
       </c>
       <c r="M72" s="21"/>
     </row>
-    <row r="73" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A73" s="16" t="s">
         <v>136</v>
       </c>
@@ -5143,7 +5140,7 @@
       </c>
       <c r="M73" s="21"/>
     </row>
-    <row r="74" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A74" s="16" t="s">
         <v>137</v>
       </c>
@@ -5180,7 +5177,7 @@
       </c>
       <c r="M74" s="21"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A75" s="16" t="s">
         <v>138</v>
       </c>
@@ -5217,7 +5214,7 @@
       </c>
       <c r="M75" s="21"/>
     </row>
-    <row r="76" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A76" s="16" t="s">
         <v>139</v>
       </c>
@@ -5252,7 +5249,7 @@
       </c>
       <c r="M76" s="21"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A77" s="13" t="s">
         <v>142</v>
       </c>
@@ -5291,7 +5288,7 @@
       </c>
       <c r="M77" s="21"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A78" s="13" t="s">
         <v>143</v>
       </c>
@@ -5330,7 +5327,7 @@
       </c>
       <c r="M78" s="21"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A79" s="13" t="s">
         <v>144</v>
       </c>
@@ -5363,7 +5360,7 @@
       </c>
       <c r="M79" s="21"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A80" s="13" t="s">
         <v>145</v>
       </c>
@@ -5398,7 +5395,7 @@
       </c>
       <c r="M80" s="21"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A81" s="13" t="s">
         <v>146</v>
       </c>
@@ -5414,7 +5411,7 @@
       <c r="E81" s="17" t="s">
         <v>406</v>
       </c>
-      <c r="F81" s="32"/>
+      <c r="F81" s="6"/>
       <c r="G81" s="15" t="s">
         <v>146</v>
       </c>
@@ -5433,7 +5430,7 @@
       </c>
       <c r="M81" s="21"/>
     </row>
-    <row r="82" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A82" s="13" t="s">
         <v>147</v>
       </c>
@@ -5470,7 +5467,7 @@
       </c>
       <c r="M82" s="21"/>
     </row>
-    <row r="83" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A83" s="13" t="s">
         <v>148</v>
       </c>
@@ -5505,7 +5502,7 @@
       </c>
       <c r="M83" s="21"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A84" s="13" t="s">
         <v>149</v>
       </c>
@@ -5538,7 +5535,7 @@
       </c>
       <c r="M84" s="21"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A85" s="28" t="s">
         <v>400</v>
       </c>
@@ -5567,7 +5564,7 @@
       <c r="L85" s="24"/>
       <c r="M85" s="23"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A86" s="28" t="s">
         <v>399</v>
       </c>
@@ -5597,13 +5594,13 @@
       <c r="L86" s="24"/>
       <c r="M86" s="23"/>
     </row>
-    <row r="99" spans="1:13" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="1:13" ht="20.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" ht="54.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="100" spans="1:13" ht="20.45" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="101" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="102" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="103" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="104" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="107" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="2"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -5618,8 +5615,8 @@
       <c r="L107" s="3"/>
       <c r="M107" s="3"/>
     </row>
-    <row r="108" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="109" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="2"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -5634,8 +5631,8 @@
       <c r="L109" s="3"/>
       <c r="M109" s="3"/>
     </row>
-    <row r="110" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="111" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="2"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -5650,7 +5647,7 @@
       <c r="L111" s="3"/>
       <c r="M111" s="3"/>
     </row>
-    <row r="113" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="2"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -5665,7 +5662,7 @@
       <c r="L113" s="3"/>
       <c r="M113" s="3"/>
     </row>
-    <row r="115" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115" s="2"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -5680,8 +5677,8 @@
       <c r="L115" s="3"/>
       <c r="M115" s="3"/>
     </row>
-    <row r="116" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="117" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A117" s="2"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -5696,12 +5693,12 @@
       <c r="L117" s="3"/>
       <c r="M117" s="3"/>
     </row>
-    <row r="118" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="130" ht="12.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="131" ht="12.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="132" ht="12.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="133" ht="12.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="134" ht="14.1" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -5803,14 +5800,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.265625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -5822,7 +5819,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5833,7 +5830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -5844,7 +5841,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -5855,7 +5852,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -5866,7 +5863,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -5877,7 +5874,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -5888,7 +5885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -5899,7 +5896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -5910,7 +5907,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -5921,7 +5918,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -5932,82 +5929,82 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -6026,12 +6023,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>

<commit_message>
test with I2C for NFC
</commit_message>
<xml_diff>
--- a/Index Produits/INDEX_EQUIPE_ILYES_CAMILLE.xlsx
+++ b/Index Produits/INDEX_EQUIPE_ILYES_CAMILLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Projet de fin de DEC\SecurityDoor\Index Produits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3aaa082c934f6d57/Documents/GitHub/SecurityDoor/Index Produits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8899210-7C81-406E-817E-6313DAF752D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{E8899210-7C81-406E-817E-6313DAF752D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F51A43D-5827-43B9-8121-5BE7C6D756E3}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LISTE" sheetId="1" r:id="rId1"/>
@@ -1390,7 +1390,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1478,10 +1478,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2217,6 +2214,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2567,11 +2568,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
@@ -5414,7 +5415,7 @@
       <c r="E81" s="17" t="s">
         <v>406</v>
       </c>
-      <c r="F81" s="32"/>
+      <c r="F81" s="6"/>
       <c r="G81" s="15" t="s">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
Updated code, added exemples and stuff
</commit_message>
<xml_diff>
--- a/Index Produits/INDEX_EQUIPE_ILYES_CAMILLE.xlsx
+++ b/Index Produits/INDEX_EQUIPE_ILYES_CAMILLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3aaa082c934f6d57/Documents/GitHub/SecurityDoor/Index Produits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{E8899210-7C81-406E-817E-6313DAF752D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F51A43D-5827-43B9-8121-5BE7C6D756E3}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{E8899210-7C81-406E-817E-6313DAF752D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C947977-907A-4AE5-8014-9B67BF9730BE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2222,7 +2222,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E488228-7BB2-48E8-8D64-0FE9665C033D}" name="Tableau13" displayName="Tableau13" ref="A5:M86" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A5:M86" xr:uid="{58943F4C-4DE4-4629-A635-9F2408F28BF2}"/>
+  <autoFilter ref="A5:M86" xr:uid="{58943F4C-4DE4-4629-A635-9F2408F28BF2}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Circuit Electrique"/>
+        <filter val="Circuit Intégré"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:M86">
     <sortCondition ref="A10:A86"/>
   </sortState>
@@ -2568,7 +2575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -2680,7 +2687,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>62</v>
       </c>
@@ -2715,7 +2722,7 @@
       </c>
       <c r="M6" s="21"/>
     </row>
-    <row r="7" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>74</v>
       </c>
@@ -2750,7 +2757,7 @@
       </c>
       <c r="M7" s="21"/>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>75</v>
       </c>
@@ -2787,7 +2794,7 @@
       </c>
       <c r="M8" s="21"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>76</v>
       </c>
@@ -2822,7 +2829,7 @@
       </c>
       <c r="M9" s="21"/>
     </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>77</v>
       </c>
@@ -2857,7 +2864,7 @@
       </c>
       <c r="M10" s="21"/>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>78</v>
       </c>
@@ -2892,7 +2899,7 @@
       </c>
       <c r="M11" s="21"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>79</v>
       </c>
@@ -2929,7 +2936,7 @@
       </c>
       <c r="M12" s="21"/>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>80</v>
       </c>
@@ -2966,7 +2973,7 @@
       </c>
       <c r="M13" s="21"/>
     </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>81</v>
       </c>
@@ -3003,7 +3010,7 @@
       </c>
       <c r="M14" s="21"/>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>82</v>
       </c>
@@ -3040,7 +3047,7 @@
       </c>
       <c r="M15" s="21"/>
     </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>83</v>
       </c>
@@ -3077,7 +3084,7 @@
       </c>
       <c r="M16" s="21"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>84</v>
       </c>
@@ -3114,7 +3121,7 @@
       </c>
       <c r="M17" s="21"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>85</v>
       </c>
@@ -3151,7 +3158,7 @@
       </c>
       <c r="M18" s="21"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>86</v>
       </c>
@@ -3186,7 +3193,7 @@
       </c>
       <c r="M19" s="21"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>87</v>
       </c>
@@ -3223,7 +3230,7 @@
       </c>
       <c r="M20" s="21"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>88</v>
       </c>
@@ -3260,7 +3267,7 @@
       </c>
       <c r="M21" s="21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>89</v>
       </c>
@@ -3297,7 +3304,7 @@
       </c>
       <c r="M22" s="21"/>
     </row>
-    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>90</v>
       </c>
@@ -3334,7 +3341,7 @@
       </c>
       <c r="M23" s="21"/>
     </row>
-    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>91</v>
       </c>
@@ -3369,7 +3376,7 @@
       </c>
       <c r="M24" s="21"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>92</v>
       </c>
@@ -3406,7 +3413,7 @@
       </c>
       <c r="M25" s="21"/>
     </row>
-    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>140</v>
       </c>
@@ -3445,7 +3452,7 @@
       </c>
       <c r="M26" s="21"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>141</v>
       </c>
@@ -3482,7 +3489,7 @@
       </c>
       <c r="M27" s="21"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>93</v>
       </c>
@@ -3519,7 +3526,7 @@
       </c>
       <c r="M28" s="21"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>94</v>
       </c>
@@ -3556,7 +3563,7 @@
       </c>
       <c r="M29" s="21"/>
     </row>
-    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>95</v>
       </c>
@@ -3593,7 +3600,7 @@
       </c>
       <c r="M30" s="21"/>
     </row>
-    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>96</v>
       </c>
@@ -3630,7 +3637,7 @@
       </c>
       <c r="M31" s="21"/>
     </row>
-    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>97</v>
       </c>
@@ -3667,7 +3674,7 @@
       </c>
       <c r="M32" s="21"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>98</v>
       </c>
@@ -3704,7 +3711,7 @@
       </c>
       <c r="M33" s="21"/>
     </row>
-    <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>67</v>
       </c>
@@ -3741,7 +3748,7 @@
       </c>
       <c r="M34" s="21"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>99</v>
       </c>
@@ -3776,7 +3783,7 @@
       </c>
       <c r="M35" s="21"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>100</v>
       </c>
@@ -3811,7 +3818,7 @@
       </c>
       <c r="M36" s="21"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>101</v>
       </c>
@@ -3846,7 +3853,7 @@
       </c>
       <c r="M37" s="21"/>
     </row>
-    <row r="38" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>102</v>
       </c>
@@ -3881,7 +3888,7 @@
       </c>
       <c r="M38" s="21"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>103</v>
       </c>
@@ -3916,7 +3923,7 @@
       </c>
       <c r="M39" s="21"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>104</v>
       </c>
@@ -4019,7 +4026,7 @@
       </c>
       <c r="M42" s="21"/>
     </row>
-    <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>107</v>
       </c>
@@ -4054,7 +4061,7 @@
       </c>
       <c r="M43" s="21"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>108</v>
       </c>
@@ -4091,7 +4098,7 @@
       </c>
       <c r="M44" s="21"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>109</v>
       </c>
@@ -4163,7 +4170,7 @@
       </c>
       <c r="M46" s="21"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>111</v>
       </c>
@@ -4200,7 +4207,7 @@
       </c>
       <c r="M47" s="21"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>112</v>
       </c>
@@ -4237,7 +4244,7 @@
       </c>
       <c r="M48" s="21"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>113</v>
       </c>
@@ -4307,7 +4314,7 @@
       </c>
       <c r="M50" s="21"/>
     </row>
-    <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>115</v>
       </c>
@@ -4344,7 +4351,7 @@
       </c>
       <c r="M51" s="21"/>
     </row>
-    <row r="52" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
         <v>116</v>
       </c>
@@ -4377,7 +4384,7 @@
       </c>
       <c r="M52" s="21"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
         <v>117</v>
       </c>
@@ -4412,7 +4419,7 @@
       </c>
       <c r="M53" s="21"/>
     </row>
-    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
         <v>118</v>
       </c>
@@ -4449,7 +4456,7 @@
       </c>
       <c r="M54" s="21"/>
     </row>
-    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
         <v>119</v>
       </c>
@@ -4486,7 +4493,7 @@
       </c>
       <c r="M55" s="21"/>
     </row>
-    <row r="56" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
         <v>120</v>
       </c>
@@ -4523,7 +4530,7 @@
       </c>
       <c r="M56" s="21"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>73</v>
       </c>
@@ -4558,7 +4565,7 @@
       </c>
       <c r="M57" s="21"/>
     </row>
-    <row r="58" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
         <v>121</v>
       </c>
@@ -4595,7 +4602,7 @@
       </c>
       <c r="M58" s="21"/>
     </row>
-    <row r="59" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
         <v>122</v>
       </c>
@@ -4632,7 +4639,7 @@
       </c>
       <c r="M59" s="21"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
         <v>123</v>
       </c>
@@ -4669,7 +4676,7 @@
       </c>
       <c r="M60" s="21"/>
     </row>
-    <row r="61" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
         <v>124</v>
       </c>
@@ -4706,7 +4713,7 @@
       </c>
       <c r="M61" s="21"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
         <v>125</v>
       </c>
@@ -4743,7 +4750,7 @@
       </c>
       <c r="M62" s="21"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
         <v>126</v>
       </c>
@@ -4780,7 +4787,7 @@
       </c>
       <c r="M63" s="21"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>127</v>
       </c>
@@ -4817,7 +4824,7 @@
       </c>
       <c r="M64" s="21"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
         <v>128</v>
       </c>
@@ -4854,7 +4861,7 @@
       </c>
       <c r="M65" s="21"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
         <v>129</v>
       </c>
@@ -4891,7 +4898,7 @@
       </c>
       <c r="M66" s="21"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
         <v>130</v>
       </c>
@@ -4928,7 +4935,7 @@
       </c>
       <c r="M67" s="21"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
         <v>131</v>
       </c>
@@ -4965,7 +4972,7 @@
       </c>
       <c r="M68" s="21"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>132</v>
       </c>
@@ -5000,7 +5007,7 @@
       </c>
       <c r="M69" s="21"/>
     </row>
-    <row r="70" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
         <v>133</v>
       </c>
@@ -5033,7 +5040,7 @@
       </c>
       <c r="M70" s="21"/>
     </row>
-    <row r="71" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
         <v>134</v>
       </c>
@@ -5070,7 +5077,7 @@
       </c>
       <c r="M71" s="21"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="16" t="s">
         <v>135</v>
       </c>
@@ -5107,7 +5114,7 @@
       </c>
       <c r="M72" s="21"/>
     </row>
-    <row r="73" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
         <v>136</v>
       </c>
@@ -5144,7 +5151,7 @@
       </c>
       <c r="M73" s="21"/>
     </row>
-    <row r="74" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
         <v>137</v>
       </c>
@@ -5181,7 +5188,7 @@
       </c>
       <c r="M74" s="21"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
         <v>138</v>
       </c>
@@ -5218,7 +5225,7 @@
       </c>
       <c r="M75" s="21"/>
     </row>
-    <row r="76" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
         <v>139</v>
       </c>
@@ -5253,7 +5260,7 @@
       </c>
       <c r="M76" s="21"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>142</v>
       </c>
@@ -5292,7 +5299,7 @@
       </c>
       <c r="M77" s="21"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>143</v>
       </c>
@@ -5331,7 +5338,7 @@
       </c>
       <c r="M78" s="21"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>144</v>
       </c>
@@ -5364,7 +5371,7 @@
       </c>
       <c r="M79" s="21"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>145</v>
       </c>
@@ -5399,7 +5406,7 @@
       </c>
       <c r="M80" s="21"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>146</v>
       </c>
@@ -5434,7 +5441,7 @@
       </c>
       <c r="M81" s="21"/>
     </row>
-    <row r="82" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>147</v>
       </c>
@@ -5471,7 +5478,7 @@
       </c>
       <c r="M82" s="21"/>
     </row>
-    <row r="83" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>148</v>
       </c>
@@ -5506,7 +5513,7 @@
       </c>
       <c r="M83" s="21"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
         <v>149</v>
       </c>

</xml_diff>

<commit_message>
Ordre dans les part Number
</commit_message>
<xml_diff>
--- a/Index Produits/INDEX_EQUIPE_ILYES_CAMILLE.xlsx
+++ b/Index Produits/INDEX_EQUIPE_ILYES_CAMILLE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projet\SecurityDoor\Index Produits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6394CBA-AF55-44E5-BD49-659322738331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3302D0-D5F8-428F-BC13-5F13BB698F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="413">
   <si>
     <t>Catégorie</t>
   </si>
@@ -1261,6 +1261,21 @@
   </si>
   <si>
     <t>CAP CER 22nF 15V 10% 0603, X7R</t>
+  </si>
+  <si>
+    <t>E00081</t>
+  </si>
+  <si>
+    <t>Motion Sensor</t>
+  </si>
+  <si>
+    <t>E00082</t>
+  </si>
+  <si>
+    <t>Temperature Sensor</t>
+  </si>
+  <si>
+    <t>PYQ 1548/7660</t>
   </si>
 </sst>
 </file>
@@ -1297,7 +1312,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1310,8 +1325,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1382,6 +1403,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1390,7 +1469,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1465,20 +1544,71 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2564,8 +2694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F89" sqref="F88:F89"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3000,7 +3130,7 @@
       <c r="M14" s="21"/>
     </row>
     <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="27" t="s">
         <v>82</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -4529,7 +4659,7 @@
       <c r="C57" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D57" s="31" t="s">
+      <c r="D57" s="28" t="s">
         <v>404</v>
       </c>
       <c r="E57" s="17" t="s">
@@ -4564,7 +4694,7 @@
       <c r="C58" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D58" s="31" t="s">
+      <c r="D58" s="28" t="s">
         <v>261</v>
       </c>
       <c r="E58" s="17" t="s">
@@ -4601,7 +4731,7 @@
       <c r="C59" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D59" s="31" t="s">
+      <c r="D59" s="28" t="s">
         <v>262</v>
       </c>
       <c r="E59" s="17" t="s">
@@ -4638,7 +4768,7 @@
       <c r="C60" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D60" s="31" t="s">
+      <c r="D60" s="28" t="s">
         <v>263</v>
       </c>
       <c r="E60" s="17" t="s">
@@ -4675,7 +4805,7 @@
       <c r="C61" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D61" s="31" t="s">
+      <c r="D61" s="28" t="s">
         <v>280</v>
       </c>
       <c r="E61" s="17" t="s">
@@ -4712,7 +4842,7 @@
       <c r="C62" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D62" s="31" t="s">
+      <c r="D62" s="28" t="s">
         <v>281</v>
       </c>
       <c r="E62" s="17" t="s">
@@ -4749,7 +4879,7 @@
       <c r="C63" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D63" s="31" t="s">
+      <c r="D63" s="28" t="s">
         <v>282</v>
       </c>
       <c r="E63" s="17" t="s">
@@ -4786,7 +4916,7 @@
       <c r="C64" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D64" s="31" t="s">
+      <c r="D64" s="28" t="s">
         <v>283</v>
       </c>
       <c r="E64" s="17" t="s">
@@ -4823,7 +4953,7 @@
       <c r="C65" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D65" s="31" t="s">
+      <c r="D65" s="28" t="s">
         <v>284</v>
       </c>
       <c r="E65" s="17" t="s">
@@ -4860,7 +4990,7 @@
       <c r="C66" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D66" s="31" t="s">
+      <c r="D66" s="28" t="s">
         <v>280</v>
       </c>
       <c r="E66" s="17" t="s">
@@ -4897,7 +5027,7 @@
       <c r="C67" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D67" s="31" t="s">
+      <c r="D67" s="28" t="s">
         <v>283</v>
       </c>
       <c r="E67" s="17" t="s">
@@ -4934,7 +5064,7 @@
       <c r="C68" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D68" s="31" t="s">
+      <c r="D68" s="28" t="s">
         <v>285</v>
       </c>
       <c r="E68" s="17" t="s">
@@ -5150,7 +5280,7 @@
       <c r="C74" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D74" s="31" t="s">
+      <c r="D74" s="28" t="s">
         <v>290</v>
       </c>
       <c r="E74" s="17" t="s">
@@ -5187,7 +5317,7 @@
       <c r="C75" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D75" s="31" t="s">
+      <c r="D75" s="28" t="s">
         <v>291</v>
       </c>
       <c r="E75" s="17" t="s">
@@ -5224,7 +5354,7 @@
       <c r="C76" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D76" s="31" t="s">
+      <c r="D76" s="28" t="s">
         <v>292</v>
       </c>
       <c r="E76" s="17" t="s">
@@ -5344,7 +5474,7 @@
         <v>200</v>
       </c>
       <c r="F79" s="6"/>
-      <c r="G79" s="29" t="s">
+      <c r="G79" s="26" t="s">
         <v>144</v>
       </c>
       <c r="H79" s="6" t="s">
@@ -5536,63 +5666,107 @@
       <c r="M84" s="21"/>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A85" s="28" t="s">
-        <v>400</v>
-      </c>
-      <c r="B85" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C85" s="24" t="s">
-        <v>398</v>
-      </c>
-      <c r="D85" s="27" t="s">
-        <v>402</v>
-      </c>
-      <c r="E85" s="24" t="s">
-        <v>401</v>
-      </c>
-      <c r="F85" s="24"/>
-      <c r="G85" s="26" t="s">
-        <v>400</v>
-      </c>
-      <c r="H85" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="I85" s="25"/>
-      <c r="J85" s="25"/>
-      <c r="K85" s="24"/>
-      <c r="L85" s="24"/>
-      <c r="M85" s="23"/>
+      <c r="A85" s="42" t="s">
+        <v>408</v>
+      </c>
+      <c r="B85" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="D85" s="46" t="s">
+        <v>412</v>
+      </c>
+      <c r="E85" s="44"/>
+      <c r="F85" s="44"/>
+      <c r="G85" s="47"/>
+      <c r="H85" s="44"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="44"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="21"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A86" s="28" t="s">
-        <v>399</v>
-      </c>
-      <c r="B86" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C86" s="24" t="s">
-        <v>398</v>
-      </c>
-      <c r="D86" s="27" t="s">
-        <v>397</v>
-      </c>
-      <c r="E86" s="24" t="s">
-        <v>396</v>
-      </c>
-      <c r="F86" s="6"/>
-      <c r="G86" s="26" t="str">
-        <f>A86</f>
-        <v>P00002</v>
-      </c>
-      <c r="H86" s="24" t="s">
-        <v>69</v>
-      </c>
+      <c r="A86" s="43" t="s">
+        <v>410</v>
+      </c>
+      <c r="B86" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="D86" s="46"/>
+      <c r="E86" s="45"/>
+      <c r="F86" s="45"/>
+      <c r="G86" s="48"/>
+      <c r="H86" s="45"/>
       <c r="I86" s="25"/>
       <c r="J86" s="25"/>
-      <c r="K86" s="24"/>
+      <c r="K86" s="45"/>
       <c r="L86" s="24"/>
       <c r="M86" s="23"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A90" s="31" t="s">
+        <v>400</v>
+      </c>
+      <c r="B90" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" s="32" t="s">
+        <v>398</v>
+      </c>
+      <c r="D90" s="33" t="s">
+        <v>402</v>
+      </c>
+      <c r="E90" s="32" t="s">
+        <v>401</v>
+      </c>
+      <c r="F90" s="32"/>
+      <c r="G90" s="34" t="s">
+        <v>400</v>
+      </c>
+      <c r="H90" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="I90" s="29"/>
+      <c r="J90" s="29"/>
+      <c r="K90" s="32"/>
+      <c r="L90" s="32"/>
+      <c r="M90" s="35"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A91" s="36" t="s">
+        <v>399</v>
+      </c>
+      <c r="B91" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C91" s="37" t="s">
+        <v>398</v>
+      </c>
+      <c r="D91" s="38" t="s">
+        <v>397</v>
+      </c>
+      <c r="E91" s="37" t="s">
+        <v>396</v>
+      </c>
+      <c r="F91" s="39"/>
+      <c r="G91" s="40" t="str">
+        <f>A91</f>
+        <v>P00002</v>
+      </c>
+      <c r="H91" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="I91" s="30"/>
+      <c r="J91" s="30"/>
+      <c r="K91" s="37"/>
+      <c r="L91" s="37"/>
+      <c r="M91" s="41"/>
     </row>
     <row r="99" spans="1:13" ht="54.95" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="100" spans="1:13" ht="20.45" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>